<commit_message>
To add the new logic and bulk upload part
</commit_message>
<xml_diff>
--- a/Client/public/Template/bulkuploadtemplate.xlsx
+++ b/Client/public/Template/bulkuploadtemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project - Internal\TaggingTool\final-dev\tagging-accelerator-v2\Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project - Internal\TaggingTool\final-dev\tagging-accelerator-v2\Client\public\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC79D1D-890D-4983-B8A1-C22485091DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AE8D76-ECE7-4B47-BB4D-DA8A4E4F88C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{805BBC22-7CA0-42DA-BA74-FBC9517B3292}"/>
+    <workbookView xWindow="2595" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{805BBC22-7CA0-42DA-BA74-FBC9517B3292}"/>
   </bookViews>
   <sheets>
     <sheet name="Bulk Upload" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Task_role</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>createdDate</t>
   </si>
@@ -50,22 +47,19 @@
     <t>task_mediatype</t>
   </si>
   <si>
-    <t>task_filename</t>
-  </si>
-  <si>
-    <t>task_filepath</t>
-  </si>
-  <si>
-    <t>task_title</t>
-  </si>
-  <si>
-    <t>profile_id</t>
-  </si>
-  <si>
-    <t>task_folder_name</t>
-  </si>
-  <si>
-    <t>project_id</t>
+    <t>project_name</t>
+  </si>
+  <si>
+    <t>numOfItemAssignToTagger</t>
+  </si>
+  <si>
+    <t>numOfItemAssignToReviewer</t>
+  </si>
+  <si>
+    <t>assignNameOftaggers</t>
+  </si>
+  <si>
+    <t>assignNameOfReviewers</t>
   </si>
 </sst>
 </file>
@@ -121,9 +115,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,7 +155,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -267,7 +261,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,7 +403,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,54 +411,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98BCF83D-46A1-4121-9F9C-79373537CD6D}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>